<commit_message>
Doan day tai lieu
</commit_message>
<xml_diff>
--- a/0.PM/ChiPhi.xlsx
+++ b/0.PM/ChiPhi.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E524FCD-C6FA-40D2-8147-DB52E26AE260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114BE50D-7110-43E4-95B0-F57EF01A9027}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$G$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$H$17</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="48">
   <si>
     <t>TT</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>Chi phí làm nộp thuế tự động đăng ký với Sở KHĐT</t>
+  </si>
+  <si>
+    <t>Thanh toán</t>
+  </si>
+  <si>
+    <t>Đã thanh toán cho Đoàn và Duy ngày 7/9/2019</t>
   </si>
 </sst>
 </file>
@@ -233,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -271,6 +277,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -611,50 +632,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="33.7265625" customWidth="1"/>
+    <col min="2" max="2" width="32.90625" customWidth="1"/>
     <col min="3" max="3" width="15.90625" customWidth="1"/>
     <col min="4" max="4" width="11.08984375" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
     <col min="6" max="6" width="16.453125" customWidth="1"/>
-    <col min="7" max="7" width="43.26953125" customWidth="1"/>
+    <col min="7" max="7" width="28.36328125" customWidth="1"/>
+    <col min="8" max="8" width="41.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="11"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G2" s="15"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F3" s="5">
         <f>SUM(F5:F254)</f>
         <v>14284000</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -674,10 +699,13 @@
         <v>2</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -696,11 +724,14 @@
       <c r="F5" s="2">
         <v>1200000</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -719,9 +750,10 @@
       <c r="F6" s="2">
         <v>200000</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G6" s="18"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -739,11 +771,12 @@
         <f>5*12*23000</f>
         <v>1380000</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="18"/>
+      <c r="H7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -762,11 +795,12 @@
       <c r="F8" s="9">
         <v>365000</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="19"/>
+      <c r="H8" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -785,11 +819,12 @@
       <c r="F9" s="9">
         <v>365000</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="19"/>
+      <c r="H9" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -808,9 +843,10 @@
       <c r="F10" s="9">
         <v>314000</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G10" s="19"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -829,11 +865,12 @@
       <c r="F11" s="9">
         <v>375000</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="19"/>
+      <c r="H11" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -852,11 +889,12 @@
       <c r="F12" s="9">
         <v>2000000</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="19"/>
+      <c r="H12" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -875,11 +913,12 @@
       <c r="F13" s="9">
         <v>200000</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="19"/>
+      <c r="H13" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -898,11 +937,12 @@
       <c r="F14" s="9">
         <v>1500000</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="19"/>
+      <c r="H14" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -921,11 +961,12 @@
       <c r="F15" s="9">
         <v>1000000</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="19"/>
+      <c r="H15" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -944,11 +985,12 @@
       <c r="F16" s="9">
         <v>365000</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="19"/>
+      <c r="H16" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -967,9 +1009,10 @@
       <c r="F17" s="14">
         <v>1500000</v>
       </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G17" s="20"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -988,11 +1031,12 @@
       <c r="F18" s="9">
         <v>365000</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="19"/>
+      <c r="H18" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -1011,11 +1055,12 @@
       <c r="F19" s="9">
         <v>365000</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="19"/>
+      <c r="H19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -1034,9 +1079,10 @@
       <c r="F20" s="14">
         <v>60000</v>
       </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G20" s="20"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -1055,9 +1101,10 @@
       <c r="F21" s="14">
         <v>1500000</v>
       </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G21" s="20"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1076,11 +1123,12 @@
       <c r="F22" s="9">
         <v>365000</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="19"/>
+      <c r="H22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -1099,11 +1147,12 @@
       <c r="F23" s="9">
         <v>365000</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="19"/>
+      <c r="H23" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -1122,14 +1171,15 @@
       <c r="F24" s="14">
         <v>500000</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="20"/>
+      <c r="H24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:G17" xr:uid="{3C114EBF-F9B7-4C6E-B13B-77DBBA155778}"/>
+  <autoFilter ref="A4:H17" xr:uid="{3C114EBF-F9B7-4C6E-B13B-77DBBA155778}"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>